<commit_message>
Updated dataset mapping, added comments
</commit_message>
<xml_diff>
--- a/maps/DataSet.xlsx
+++ b/maps/DataSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nictiz\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C59406-1F3F-4540-8C42-970520E9714E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5D3727-11CC-4120-B9A4-3E7BBAE359F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
+    <workbookView xWindow="-13500" yWindow="-21600" windowWidth="34605" windowHeight="20985" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8631DB2A-343D-442B-A304-5E36E8950659}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B24"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,9 +546,6 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -651,11 +648,16 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>